<commit_message>
algorith d'insertion et supression dans l'arbre
</commit_message>
<xml_diff>
--- a/METADATA - ADHESION.xlsx
+++ b/METADATA - ADHESION.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Civilité</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>Café-Cacao</t>
+  </si>
+  <si>
+    <t>Lezou Marman</t>
+  </si>
+  <si>
+    <t>Kouassi Linda</t>
+  </si>
+  <si>
+    <t>lm@bbmlm.ci</t>
+  </si>
+  <si>
+    <t>kl@bbmlm.ci</t>
   </si>
 </sst>
 </file>
@@ -152,7 +164,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -164,10 +176,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -199,15 +211,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G2" totalsRowShown="0" headerRowDxfId="8" dataDxfId="2">
-  <autoFilter ref="A1:G2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G4"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Civilité" dataDxfId="7"/>
-    <tableColumn id="2" name="Nom &amp; Prénoms" dataDxfId="6"/>
-    <tableColumn id="7" name="Corporation" dataDxfId="0"/>
-    <tableColumn id="3" name="Date de Naissance" dataDxfId="1"/>
-    <tableColumn id="4" name="Email" dataDxfId="5"/>
-    <tableColumn id="5" name="Nature" dataDxfId="4"/>
+    <tableColumn id="1" name="Civilité" dataDxfId="6"/>
+    <tableColumn id="2" name="Nom &amp; Prénoms" dataDxfId="5"/>
+    <tableColumn id="7" name="Corporation" dataDxfId="4"/>
+    <tableColumn id="3" name="Date de Naissance" dataDxfId="2"/>
+    <tableColumn id="4" name="Email" dataDxfId="0"/>
+    <tableColumn id="5" name="Nature" dataDxfId="1"/>
     <tableColumn id="6" name="Code Parrain" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -534,7 +546,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +598,7 @@
       <c r="D2" s="3">
         <v>28774</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -596,8 +608,52 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>35350</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>33159</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="5" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -620,23 +676,24 @@
     <row r="24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
       <formula1>civility</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
       <formula1>nature</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4">
       <formula1>corporation</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
deplacement dans l'arbre terminé
</commit_message>
<xml_diff>
--- a/METADATA - ADHESION.xlsx
+++ b/METADATA - ADHESION.xlsx
@@ -71,15 +71,6 @@
     <t>NOVUS CUSTOMER</t>
   </si>
   <si>
-    <t>Blé Brice Uriel</t>
-  </si>
-  <si>
-    <t>bb@bbmlm.ci</t>
-  </si>
-  <si>
-    <t>ZDdkNDNkMDJjNjBhZDg1NTc5YThiNT</t>
-  </si>
-  <si>
     <t>Corporation</t>
   </si>
   <si>
@@ -98,16 +89,25 @@
     <t>Café-Cacao</t>
   </si>
   <si>
-    <t>Lezou Marman</t>
-  </si>
-  <si>
-    <t>Kouassi Linda</t>
-  </si>
-  <si>
-    <t>lm@bbmlm.ci</t>
-  </si>
-  <si>
-    <t>kl@bbmlm.ci</t>
+    <t>bb@bbmlm.ci19</t>
+  </si>
+  <si>
+    <t>bb@bbmlm.ci20</t>
+  </si>
+  <si>
+    <t>bb@bbmlm.ci21</t>
+  </si>
+  <si>
+    <t>Paquebot</t>
+  </si>
+  <si>
+    <t>Voilier</t>
+  </si>
+  <si>
+    <t>Yzc2MDU5NmU4N2MyZDdkNDIwZjIwNz</t>
+  </si>
+  <si>
+    <t>Planche à Voile</t>
   </si>
 </sst>
 </file>
@@ -179,10 +179,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -217,10 +217,10 @@
     <tableColumn id="1" name="Civilité" dataDxfId="6"/>
     <tableColumn id="2" name="Nom &amp; Prénoms" dataDxfId="5"/>
     <tableColumn id="7" name="Corporation" dataDxfId="4"/>
-    <tableColumn id="3" name="Date de Naissance" dataDxfId="2"/>
-    <tableColumn id="4" name="Email" dataDxfId="0"/>
+    <tableColumn id="3" name="Date de Naissance" dataDxfId="3"/>
+    <tableColumn id="4" name="Email" dataDxfId="2"/>
     <tableColumn id="5" name="Nature" dataDxfId="1"/>
-    <tableColumn id="6" name="Code Parrain" dataDxfId="3"/>
+    <tableColumn id="6" name="Code Parrain" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -543,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -590,22 +590,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3">
         <v>28774</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -616,42 +616,42 @@
         <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>35350</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
-        <v>33159</v>
+        <v>35351</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -663,17 +663,6 @@
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
@@ -687,13 +676,14 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2" display="bb@bbmlm.ci19"/>
+    <hyperlink ref="E4" r:id="rId3" display="bb@bbmlm.ci19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -720,7 +710,7 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -731,7 +721,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -742,7 +732,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -753,7 +743,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -761,7 +751,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,7 +759,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>